<commit_message>
fix: invalid PERC questions scoring rules
Add a fix that will result in an error being raised if any of the scoring rules on a PERC question are missing the '%' sign.
</commit_message>
<xml_diff>
--- a/resources/Mentorship Checklist Metadata v1.0.0.xlsx
+++ b/resources/Mentorship Checklist Metadata v1.0.0.xlsx
@@ -10,15 +10,15 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">Questions!$E$1:$E$979</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_C5F29CBF_5FE9_4096_80E9_02EA8DB0AD22_.wvu.FilterData">Questions!$A$1:$I$150</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_F860D748_7807_42AC_B71A_9264A00B0DCF_.wvu.FilterData">Questions!$A$1:$I$433</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_FBA27144_7885_4740_993D_B6F10E6EC409_.wvu.FilterData">Questions!$A$1:$I$616</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_A5839548_3753_4B04_B023_4659710468EB_.wvu.FilterData">Questions!$A$1:$I$616</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_AD5D5E5E_F40E_4BAA_9457_C4BE69E75B6C_.wvu.FilterData">Questions!$A$1:$I$150</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_4F52AC96_6374_4985_9D2B_CA8CE7EE4140_.wvu.FilterData">Questions!$A$1:$I$433</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FBA27144-7885-4740-993D-B6F10E6EC409}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C5F29CBF-5FE9-4096-80E9-02EA8DB0AD22}" name="Filter 3"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F860D748-7807-42AC-B71A-9264A00B0DCF}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A5839548-3753-4B04-B023-4659710468EB}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{AD5D5E5E-F40E-4BAA-9457-C4BE69E75B6C}" name="Filter 3"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4F52AC96-6374-4985-9D2B-CA8CE7EE4140}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1344,7 +1344,7 @@
     <t>C1_14_03_NUM</t>
   </si>
   <si>
-    <t>Number of PNC mothers with</t>
+    <t xml:space="preserve">Number of PNC mothers on / started on modern family planning </t>
   </si>
   <si>
     <t>C1_14_03_DEN</t>
@@ -5454,7 +5454,7 @@
     <t>Review MOH 717 for the workload</t>
   </si>
   <si>
-    <t xml:space="preserve">If &lt;50% = Red; If ≥ 50 and &lt; 80% = Yellow; If ≥ 80% = Green
+    <t xml:space="preserve">If &lt;50% = Red; If ≥ 50% and &lt; 80% = Yellow; If ≥ 80% = Green
 </t>
   </si>
   <si>
@@ -5476,7 +5476,7 @@
     <t>Review the percentage (%) of patients screened and presumed to have TB who have a documented HIV test results in the presumptive TB register in the last 3 months</t>
   </si>
   <si>
-    <t>If &lt;70% = Red; If ≥ 70 and &lt;90% = Yellow; If ≥ 90% = Green</t>
+    <t>If &lt;70% = Red; If ≥ 70% and &lt;90% = Yellow; If ≥ 90% = Green</t>
   </si>
   <si>
     <t>C11_01_05_NUM</t>
@@ -5542,7 +5542,7 @@
     <t>For all the clients who tested HIV negative in the last 1 month in the facility, what percentage of the negatives have been linked to Prep?</t>
   </si>
   <si>
-    <t xml:space="preserve">If &lt;5% = Red; If ≥ 5 and &lt;15% = Yellow; If ≥ 15% = Green
+    <t xml:space="preserve">If &lt;5% = Red; If ≥ 5% and &lt;15% = Yellow; If ≥ 15% = Green
 </t>
   </si>
   <si>
@@ -6080,7 +6080,7 @@
     <t>Review the index contacts testing uptake by checking the percentage of elicited contacts (both sexual partners and biological children) who have been offered HIV testing in the past 3 months</t>
   </si>
   <si>
-    <t>If &lt;60% = Red; If ≥ 60 and &lt;90% = Yellow; If ≥ 90% = Green</t>
+    <t>If &lt;60% = Red; If ≥ 60% and &lt;90% = Yellow; If ≥ 90% = Green</t>
   </si>
   <si>
     <t>C13_01_07_NUM</t>
@@ -39728,13 +39728,13 @@
   </sheetData>
   <autoFilter ref="$E$1:$E$979"/>
   <customSheetViews>
-    <customSheetView guid="{F860D748-7807-42AC-B71A-9264A00B0DCF}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4F52AC96-6374-4985-9D2B-CA8CE7EE4140}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$I$433"/>
     </customSheetView>
-    <customSheetView guid="{FBA27144-7885-4740-993D-B6F10E6EC409}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A5839548-3753-4B04-B023-4659710468EB}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$I$616"/>
     </customSheetView>
-    <customSheetView guid="{C5F29CBF-5FE9-4096-80E9-02EA8DB0AD22}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AD5D5E5E-F40E-4BAA-9457-C4BE69E75B6C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$I$150"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
fix: invalid PERC questions scoring rules (#2)
Add a fix that will result in an error being raised if any of the scoring rules on a PERC question are missing the '%' sign.
</commit_message>
<xml_diff>
--- a/resources/Mentorship Checklist Metadata v1.0.0.xlsx
+++ b/resources/Mentorship Checklist Metadata v1.0.0.xlsx
@@ -10,15 +10,15 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">Questions!$E$1:$E$979</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_C5F29CBF_5FE9_4096_80E9_02EA8DB0AD22_.wvu.FilterData">Questions!$A$1:$I$150</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_F860D748_7807_42AC_B71A_9264A00B0DCF_.wvu.FilterData">Questions!$A$1:$I$433</definedName>
-    <definedName hidden="1" localSheetId="2" name="Z_FBA27144_7885_4740_993D_B6F10E6EC409_.wvu.FilterData">Questions!$A$1:$I$616</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_A5839548_3753_4B04_B023_4659710468EB_.wvu.FilterData">Questions!$A$1:$I$616</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_AD5D5E5E_F40E_4BAA_9457_C4BE69E75B6C_.wvu.FilterData">Questions!$A$1:$I$150</definedName>
+    <definedName hidden="1" localSheetId="2" name="Z_4F52AC96_6374_4985_9D2B_CA8CE7EE4140_.wvu.FilterData">Questions!$A$1:$I$433</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FBA27144-7885-4740-993D-B6F10E6EC409}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C5F29CBF-5FE9-4096-80E9-02EA8DB0AD22}" name="Filter 3"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F860D748-7807-42AC-B71A-9264A00B0DCF}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A5839548-3753-4B04-B023-4659710468EB}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{AD5D5E5E-F40E-4BAA-9457-C4BE69E75B6C}" name="Filter 3"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4F52AC96-6374-4985-9D2B-CA8CE7EE4140}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1344,7 +1344,7 @@
     <t>C1_14_03_NUM</t>
   </si>
   <si>
-    <t>Number of PNC mothers with</t>
+    <t xml:space="preserve">Number of PNC mothers on / started on modern family planning </t>
   </si>
   <si>
     <t>C1_14_03_DEN</t>
@@ -5454,7 +5454,7 @@
     <t>Review MOH 717 for the workload</t>
   </si>
   <si>
-    <t xml:space="preserve">If &lt;50% = Red; If ≥ 50 and &lt; 80% = Yellow; If ≥ 80% = Green
+    <t xml:space="preserve">If &lt;50% = Red; If ≥ 50% and &lt; 80% = Yellow; If ≥ 80% = Green
 </t>
   </si>
   <si>
@@ -5476,7 +5476,7 @@
     <t>Review the percentage (%) of patients screened and presumed to have TB who have a documented HIV test results in the presumptive TB register in the last 3 months</t>
   </si>
   <si>
-    <t>If &lt;70% = Red; If ≥ 70 and &lt;90% = Yellow; If ≥ 90% = Green</t>
+    <t>If &lt;70% = Red; If ≥ 70% and &lt;90% = Yellow; If ≥ 90% = Green</t>
   </si>
   <si>
     <t>C11_01_05_NUM</t>
@@ -5542,7 +5542,7 @@
     <t>For all the clients who tested HIV negative in the last 1 month in the facility, what percentage of the negatives have been linked to Prep?</t>
   </si>
   <si>
-    <t xml:space="preserve">If &lt;5% = Red; If ≥ 5 and &lt;15% = Yellow; If ≥ 15% = Green
+    <t xml:space="preserve">If &lt;5% = Red; If ≥ 5% and &lt;15% = Yellow; If ≥ 15% = Green
 </t>
   </si>
   <si>
@@ -6080,7 +6080,7 @@
     <t>Review the index contacts testing uptake by checking the percentage of elicited contacts (both sexual partners and biological children) who have been offered HIV testing in the past 3 months</t>
   </si>
   <si>
-    <t>If &lt;60% = Red; If ≥ 60 and &lt;90% = Yellow; If ≥ 90% = Green</t>
+    <t>If &lt;60% = Red; If ≥ 60% and &lt;90% = Yellow; If ≥ 90% = Green</t>
   </si>
   <si>
     <t>C13_01_07_NUM</t>
@@ -39728,13 +39728,13 @@
   </sheetData>
   <autoFilter ref="$E$1:$E$979"/>
   <customSheetViews>
-    <customSheetView guid="{F860D748-7807-42AC-B71A-9264A00B0DCF}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4F52AC96-6374-4985-9D2B-CA8CE7EE4140}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$I$433"/>
     </customSheetView>
-    <customSheetView guid="{FBA27144-7885-4740-993D-B6F10E6EC409}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A5839548-3753-4B04-B023-4659710468EB}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$I$616"/>
     </customSheetView>
-    <customSheetView guid="{C5F29CBF-5FE9-4096-80E9-02EA8DB0AD22}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AD5D5E5E-F40E-4BAA-9457-C4BE69E75B6C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$I$150"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>